<commit_message>
Updated incorrect WIDTH calculation.
</commit_message>
<xml_diff>
--- a/Slice_Data_with_OFFSET.xlsx
+++ b/Slice_Data_with_OFFSET.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wendy\Documents\VBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wendy\Documents\YT_Rustige_Oom\Excel-Formulas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760F5561-2C50-44A6-9338-C48D90EC6F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9FE78F0-6C05-4D2A-ADD2-36485F19A9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1D0E0CD7-713F-4346-AAF1-8C4C8B5051DF}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="SLICE">_xlfn.LAMBDA(_xlpm.source_data,_xlpm.row_start,_xlpm.row_end,_xlpm.column_start,_xlpm.column_end, OFFSET(_xlpm.source_data, IF(OR(ISBLANK(_xlpm.row_start), TRIM(_xlpm.row_start)=""), 1, _xlpm.row_start) - 1, IF(OR(ISBLANK(_xlpm.column_start), TRIM(_xlpm.column_start)=""), 1, _xlpm.column_start) - 1, IF(OR(ISBLANK(_xlpm.row_end), TRIM(_xlpm.row_end)=""), ROWS(_xlpm.source_data), IF(AND(_xlpm.row_end&lt;0, _xlpm.row_end&gt;= -1*ROWS(_xlpm.source_data)), ROWS(_xlpm.source_data) + _xlpm.row_end + 1, IF(AND(_xlpm.row_end&gt;=1, _xlpm.row_end&lt;=ROWS(_xlpm.source_data)), _xlpm.row_end, NA()))) - IF(OR(ISBLANK(_xlpm.row_start), TRIM(_xlpm.row_start)=""), 1, _xlpm.row_start) + 1, IF(OR(ISBLANK(_xlpm.column_end), TRIM(_xlpm.column_end)=""), ROWS(_xlpm.source_data), IF(AND(_xlpm.column_end&lt;0, _xlpm.column_end&gt;= -1*ROWS(_xlpm.source_data)), ROWS(_xlpm.source_data) + _xlpm.column_end + 1, IF(AND(_xlpm.column_end&gt;=1, _xlpm.column_end&lt;=ROWS(_xlpm.source_data)), _xlpm.column_end, NA()))) - IF(OR(ISBLANK(_xlpm.column_start), TRIM(_xlpm.column_start)=""), 1, _xlpm.column_start) + 1))</definedName>
+    <definedName name="SLICE">_xlfn.LAMBDA(_xlpm.source_data,_xlpm.row_start,_xlpm.row_end,_xlpm.column_start,_xlpm.column_end, OFFSET(_xlpm.source_data, IF(OR(ISBLANK(_xlpm.row_start), TRIM(_xlpm.row_start)=""), 1, _xlpm.row_start) - 1, IF(OR(ISBLANK(_xlpm.column_start), TRIM(_xlpm.column_start)=""), 1, _xlpm.column_start) - 1, IF(OR(ISBLANK(_xlpm.row_end), TRIM(_xlpm.row_end)=""), ROWS(_xlpm.source_data), IF(AND(_xlpm.row_end&lt;0, _xlpm.row_end&gt;= -1*ROWS(_xlpm.source_data)), ROWS(_xlpm.source_data) + _xlpm.row_end + 1, IF(AND(_xlpm.row_end&gt;=1, _xlpm.row_end&lt;=ROWS(_xlpm.source_data)), _xlpm.row_end, NA()))) - IF(OR(ISBLANK(_xlpm.row_start), TRIM(_xlpm.row_start)=""), 1, _xlpm.row_start) + 1, IF(OR(ISBLANK(_xlpm.column_end), TRIM(_xlpm.column_end)=""), COLUMNS(_xlpm.source_data), IF(AND(_xlpm.column_end&lt;0, _xlpm.column_end&gt;= -1*COLUMNS(_xlpm.source_data)), COLUMNS(_xlpm.source_data) + _xlpm.column_end + 1, IF(AND(_xlpm.column_end&gt;=1, _xlpm.column_end&lt;=COLUMNS(_xlpm.source_data)), _xlpm.column_end, NA()))) - IF(OR(ISBLANK(_xlpm.column_start), TRIM(_xlpm.column_start)=""), 1, _xlpm.column_start) + 1))</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -446,7 +446,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>